<commit_message>
Ticket #28173: Test files for ParseExcel.
</commit_message>
<xml_diff>
--- a/com.top_logic.demo/src/main/webapp/WEB-INF/test/fixtures/ParseExcelTestFile.xlsx
+++ b/com.top_logic.demo/src/main/webapp/WEB-INF/test/fixtures/ParseExcelTestFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbe.BOS\development\TL_git\tl-engine\com.top_logic.demo\src\main\webapp\WEB-INF\test\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990E8A8E-E53E-4C1F-AE59-6EAC536AE6AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF366E00-2E2F-4868-9AD9-8394EF5C8FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="705" windowWidth="16350" windowHeight="9555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10860" yWindow="4395" windowWidth="16350" windowHeight="9120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datentypen" sheetId="1" r:id="rId1"/>
@@ -212,19 +212,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -509,7 +509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -685,39 +685,39 @@
       <c r="D3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6" t="s">
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="7" t="s">
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="3:11" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="7" t="s">
         <v>27</v>
       </c>
       <c r="K4" s="4"/>
@@ -831,9 +831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{538BB5FA-88A7-4C3D-8C46-2A70E2EE21A6}">
   <dimension ref="C3:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -841,43 +839,43 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:11" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9" t="s">
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
     </row>
     <row r="4" spans="3:11" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="8" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>